<commit_message>
04: Updated excel data
</commit_message>
<xml_diff>
--- a/04_RozpadPlazmatu/data/RozpadPlazmatu.xlsx
+++ b/04_RozpadPlazmatu/data/RozpadPlazmatu.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\04_RozpadPlazmatu\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAF29FE-AA9E-45D2-9AC8-86A8C8A04C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="19176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="19">
   <si>
     <t>RozpadPlazmatu</t>
   </si>
@@ -74,13 +68,31 @@
   <si>
     <t>ln n</t>
   </si>
+  <si>
+    <t>R [m]</t>
+  </si>
+  <si>
+    <t>R' [m]</t>
+  </si>
+  <si>
+    <t>V/V'</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>e0</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.00000000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -121,13 +133,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -143,7 +156,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -185,7 +198,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,26 +231,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,23 +266,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -462,32 +441,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF128"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T44" sqref="T44"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ39" sqref="AJ39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.28515625" customWidth="1"/>
-    <col min="29" max="29" width="16.5703125" customWidth="1"/>
+    <col min="24" max="24" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.33203125" customWidth="1"/>
+    <col min="29" max="29" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -495,7 +475,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -538,8 +518,11 @@
       <c r="AF4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -588,8 +571,12 @@
         <f>LN(AD5)</f>
         <v>25.278932798864712</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH5" s="3">
+        <f>0.271/0.64 * $U$11 * AC5 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>23391714.358266436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -607,11 +594,11 @@
         <v>2.7713399999999999</v>
       </c>
       <c r="AB6">
-        <f t="shared" ref="AB6:AB37" si="0">Z6/1000000</f>
+        <f t="shared" ref="AB6:AB18" si="0">Z6/1000000</f>
         <v>9.5000000000000005E-5</v>
       </c>
       <c r="AC6">
-        <f t="shared" ref="AC6:AC19" si="1">AA6-$X$5</f>
+        <f t="shared" ref="AC6:AC18" si="1">AA6-$X$5</f>
         <v>4.0359999999999729E-2</v>
       </c>
       <c r="AD6">
@@ -623,11 +610,15 @@
         <v>1.1344062326741826E-11</v>
       </c>
       <c r="AF6">
-        <f t="shared" ref="AF6:AF19" si="3">LN(AD6)</f>
+        <f t="shared" ref="AF6:AF18" si="3">LN(AD6)</f>
         <v>25.202326651906528</v>
       </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH6" s="3">
+        <f t="shared" ref="AH6:AH19" si="4">0.271/0.64 * $U$11 * AC6 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>22870387.390979342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1</v>
       </c>
@@ -692,7 +683,7 @@
         <v>3.8059999999999761E-2</v>
       </c>
       <c r="AD7">
-        <f t="shared" ref="AD6:AD37" si="4">(0.271*0.04^2*AC7*1000000000*8*PI()^2*8.854*0.000000000001*9.107*1E-31)/(0.64*0.009^2*(1.602*0.0000000000000000001)^2*(Z7/1000000))</f>
+        <f t="shared" ref="AD7:AD18" si="5">(0.271*0.04^2*AC7*1000000000*8*PI()^2*8.854*0.000000000001*9.107*1E-31)/(0.64*0.009^2*(1.602*0.0000000000000000001)^2*(Z7/1000000))</f>
         <v>75211340400.609711</v>
       </c>
       <c r="AE7">
@@ -703,8 +694,12 @@
         <f t="shared" si="3"/>
         <v>25.043567859732143</v>
       </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH7" s="3">
+        <f t="shared" si="4"/>
+        <v>21567069.972761996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -768,6 +763,12 @@
         <f>O8+120</f>
         <v>890</v>
       </c>
+      <c r="U8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V8" t="s">
+        <v>14</v>
+      </c>
       <c r="Y8">
         <v>4</v>
       </c>
@@ -787,7 +788,7 @@
         <v>3.5320000000000018E-2</v>
       </c>
       <c r="AD8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>61072161720.463974</v>
       </c>
       <c r="AE8">
@@ -798,8 +799,12 @@
         <f t="shared" si="3"/>
         <v>24.835321980975383</v>
       </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH8" s="3">
+        <f t="shared" si="4"/>
+        <v>20014422.265842322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -847,6 +852,14 @@
       </c>
       <c r="P9">
         <v>2.7332399999999999</v>
+      </c>
+      <c r="U9">
+        <f>0.04</f>
+        <v>0.04</v>
+      </c>
+      <c r="V9">
+        <f>0.009</f>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="Y9">
         <v>5</v>
@@ -867,7 +880,7 @@
         <v>3.2429999999999737E-2</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>48064314947.289185</v>
       </c>
       <c r="AE9">
@@ -878,8 +891,21 @@
         <f t="shared" si="3"/>
         <v>24.595805845731583</v>
       </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH9" s="3">
+        <f t="shared" si="4"/>
+        <v>18376775.596864697</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+      <c r="U10" t="s">
+        <v>15</v>
+      </c>
+      <c r="V10" t="s">
+        <v>17</v>
+      </c>
+      <c r="W10" t="s">
+        <v>18</v>
+      </c>
       <c r="Y10">
         <v>6</v>
       </c>
@@ -899,7 +925,7 @@
         <v>2.8479999999999617E-2</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34761211760.684616</v>
       </c>
       <c r="AE10">
@@ -910,13 +936,27 @@
         <f t="shared" si="3"/>
         <v>24.27176799751517</v>
       </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH10" s="3">
+        <f t="shared" si="4"/>
+        <v>16138469.596013067</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="1">
         <v>20</v>
+      </c>
+      <c r="U11">
+        <f>U9^2/V9^2</f>
+        <v>19.753086419753089</v>
+      </c>
+      <c r="V11" s="3">
+        <v>8.8539999999999992E-12</v>
+      </c>
+      <c r="W11" s="3">
+        <v>9.1070000000000006E-31</v>
       </c>
       <c r="Y11">
         <v>7</v>
@@ -937,7 +977,7 @@
         <v>2.3939999999999628E-2</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23654223452.319756</v>
       </c>
       <c r="AE11">
@@ -948,12 +988,19 @@
         <f t="shared" si="3"/>
         <v>23.886807517434011</v>
       </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH11" s="3">
+        <f t="shared" si="4"/>
+        <v>13565834.344401404</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="U12" t="s">
         <v>16</v>
       </c>
       <c r="Y12">
@@ -975,7 +1022,7 @@
         <v>1.9649999999999945E-2</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>15681696721.932833</v>
       </c>
       <c r="AE12">
@@ -986,13 +1033,20 @@
         <f t="shared" si="3"/>
         <v>23.475760055321409</v>
       </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH12" s="3">
+        <f t="shared" si="4"/>
+        <v>11134864.029552674</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13">
         <v>880</v>
+      </c>
+      <c r="U13" s="3">
+        <v>1.602E-19</v>
       </c>
       <c r="Y13">
         <v>9</v>
@@ -1013,7 +1067,7 @@
         <v>1.5479999999999716E-2</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10037482978.122498</v>
       </c>
       <c r="AE13">
@@ -1024,8 +1078,12 @@
         <f t="shared" si="3"/>
         <v>23.029592220389461</v>
       </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH13" s="3">
+        <f t="shared" si="4"/>
+        <v>8771892.8843497559</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1051,7 +1109,7 @@
         <v>1.1529999999999596E-2</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6103052193.0997467</v>
       </c>
       <c r="AE14">
@@ -1062,8 +1120,12 @@
         <f t="shared" si="3"/>
         <v>22.532054842512139</v>
       </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH14" s="3">
+        <f t="shared" si="4"/>
+        <v>6533586.8834981276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1</v>
       </c>
@@ -1128,7 +1190,7 @@
         <v>8.6299999999996935E-3</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3793784351.6487403</v>
       </c>
       <c r="AE15">
@@ -1139,8 +1201,12 @@
         <f t="shared" si="3"/>
         <v>22.056629867531417</v>
       </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH15" s="3">
+        <f t="shared" si="4"/>
+        <v>4890273.6170502007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1223,7 +1289,7 @@
         <v>6.1599999999999433E-3</v>
       </c>
       <c r="AD16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2282425069.9606929</v>
       </c>
       <c r="AE16">
@@ -1234,8 +1300,12 @@
         <f t="shared" si="3"/>
         <v>21.548504341837894</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH16" s="3">
+        <f t="shared" si="4"/>
+        <v>3490624.0418343013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1303,7 +1373,7 @@
         <v>4.269999999999996E-3</v>
       </c>
       <c r="AD17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1342418050.7895644</v>
       </c>
       <c r="AE17">
@@ -1314,8 +1384,12 @@
         <f t="shared" si="3"/>
         <v>21.017738340241731</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH17" s="3">
+        <f t="shared" si="4"/>
+        <v>2419637.1199078881</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y18">
         <v>14</v>
       </c>
@@ -1335,7 +1409,7 @@
         <v>2.9499999999997861E-3</v>
       </c>
       <c r="AD18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>794941435.22828996</v>
       </c>
       <c r="AE18">
@@ -1346,8 +1420,12 @@
         <f t="shared" si="3"/>
         <v>20.493779003525596</v>
       </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH18" s="3">
+        <f t="shared" si="4"/>
+        <v>1671646.2538004122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y19">
         <v>15</v>
       </c>
@@ -1359,15 +1437,15 @@
         <v>2.7332399999999999</v>
       </c>
       <c r="AB19">
-        <f t="shared" ref="AB19:AB82" si="5">Z19/1000000</f>
+        <f t="shared" ref="AB19:AB82" si="6">Z19/1000000</f>
         <v>8.8999999999999995E-4</v>
       </c>
       <c r="AC19">
-        <f t="shared" ref="AC19:AC82" si="6">AA19-$X$5</f>
+        <f t="shared" ref="AC19:AC82" si="7">AA19-$X$5</f>
         <v>2.2599999999997067E-3</v>
       </c>
       <c r="AD19">
-        <f t="shared" ref="AD19:AD82" si="7">(0.271*0.04^2*AC19*1000000000*8*PI()^2*8.854*0.000000000001*9.107*1E-31)/(0.64*0.009^2*(1.602*0.0000000000000000001)^2*(Z19/1000000))</f>
+        <f t="shared" ref="AD19:AD82" si="8">(0.271*0.04^2*AC19*1000000000*8*PI()^2*8.854*0.000000000001*9.107*1E-31)/(0.64*0.009^2*(1.602*0.0000000000000000001)^2*(Z19/1000000))</f>
         <v>526892814.92446816</v>
       </c>
       <c r="AE19">
@@ -1375,11 +1453,15 @@
         <v>1.8979192193830794E-9</v>
       </c>
       <c r="AF19">
-        <f t="shared" ref="AF19:AF82" si="8">LN(AD19)</f>
+        <f t="shared" ref="AF19:AF82" si="9">LN(AD19)</f>
         <v>20.082507698579548</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH19" s="3">
+        <f t="shared" si="4"/>
+        <v>1280651.0283351575</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1387,7 +1469,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1395,7 +1477,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1435,8 +1517,11 @@
       <c r="AF22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1466,15 +1551,15 @@
         <v>2.77251</v>
       </c>
       <c r="AB23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AC23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.1529999999999845E-2</v>
       </c>
       <c r="AD23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>538574506565.15948</v>
       </c>
       <c r="AE23">
@@ -1482,11 +1567,15 @@
         <v>1.8567533141842371E-12</v>
       </c>
       <c r="AF23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>27.012191683424547</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH23" s="3">
+        <f>0.271/0.64 * $U$11 * AC23 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>23533379.295029119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1</v>
       </c>
@@ -1546,15 +1635,15 @@
         <v>2.7698299999999998</v>
       </c>
       <c r="AB24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="AC24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.8849999999999607E-2</v>
       </c>
       <c r="AD24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>403055518036.24011</v>
       </c>
       <c r="AE24">
@@ -1562,11 +1651,15 @@
         <v>2.4810477843652461E-12</v>
       </c>
       <c r="AF24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>26.722340151281326</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH24" s="3">
+        <f t="shared" ref="AH24:AH37" si="10">0.271/0.64 * $U$11 * AC24 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>22014731.172932219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1645,15 +1738,15 @@
         <v>2.7686199999999999</v>
       </c>
       <c r="AB25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="AC25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.7639999999999674E-2</v>
       </c>
       <c r="AD25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>260334786767.63788</v>
       </c>
       <c r="AE25">
@@ -1661,11 +1754,15 @@
         <v>3.8412077479778034E-12</v>
       </c>
       <c r="AF25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>26.285234281076683</v>
       </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH25" s="3">
+        <f t="shared" si="10"/>
+        <v>21329072.879000518</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1728,15 +1825,15 @@
         <v>2.7656499999999999</v>
       </c>
       <c r="AB26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000000000000003E-5</v>
       </c>
       <c r="AC26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.4669999999999757E-2</v>
       </c>
       <c r="AD26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>159861974091.99472</v>
       </c>
       <c r="AE26">
@@ -1744,11 +1841,15 @@
         <v>6.2553962922072797E-12</v>
       </c>
       <c r="AF26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25.797576617948273</v>
       </c>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH26" s="3">
+        <f t="shared" si="10"/>
+        <v>19646093.430259012</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y27">
         <v>5</v>
       </c>
@@ -1760,15 +1861,15 @@
         <v>2.7625600000000001</v>
       </c>
       <c r="AB27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.4999999999999994E-5</v>
       </c>
       <c r="AC27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.1579999999999941E-2</v>
       </c>
       <c r="AD27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100809767425.67722</v>
       </c>
       <c r="AE27">
@@ -1776,11 +1877,15 @@
         <v>9.9196737135343328E-12</v>
       </c>
       <c r="AF27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25.336501086953525</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH27" s="3">
+        <f t="shared" si="10"/>
+        <v>17895114.811871435</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y28">
         <v>6</v>
       </c>
@@ -1792,15 +1897,15 @@
         <v>2.7574800000000002</v>
       </c>
       <c r="AB28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.5000000000000005E-5</v>
       </c>
       <c r="AC28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.6499999999999968E-2</v>
       </c>
       <c r="AD28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>57879678807.616104</v>
       </c>
       <c r="AE28">
@@ -1808,11 +1913,15 @@
         <v>1.7277220962539532E-11</v>
       </c>
       <c r="AF28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24.781632189413305</v>
       </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH28" s="3">
+        <f t="shared" si="10"/>
+        <v>15016483.296852231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1830,15 +1939,15 @@
         <v>2.75237</v>
       </c>
       <c r="AB29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.34E-4</v>
       </c>
       <c r="AC29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1389999999999798E-2</v>
       </c>
       <c r="AD29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>33121487277.10936</v>
       </c>
       <c r="AE29">
@@ -1846,11 +1955,15 @@
         <v>3.0191880927131903E-11</v>
       </c>
       <c r="AF29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24.223448071165063</v>
       </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH29" s="3">
+        <f t="shared" si="10"/>
+        <v>12120851.989421375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -1868,15 +1981,15 @@
         <v>2.7461700000000002</v>
       </c>
       <c r="AB30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.84E-4</v>
       </c>
       <c r="AC30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.5190000000000037E-2</v>
       </c>
       <c r="AD30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>17129464828.410736</v>
       </c>
       <c r="AE30">
@@ -1884,11 +1997,15 @@
         <v>5.8378940032114219E-11</v>
       </c>
       <c r="AF30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>23.564065907020368</v>
       </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH30" s="3">
+        <f t="shared" si="10"/>
+        <v>8607561.5577051379</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1906,15 +2023,15 @@
         <v>2.7423600000000001</v>
       </c>
       <c r="AB31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.4399999999999999E-4</v>
       </c>
       <c r="AC31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1379999999999946E-2</v>
       </c>
       <c r="AD31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9677346235.5263767</v>
       </c>
       <c r="AE31">
@@ -1922,11 +2039,15 @@
         <v>1.0333411409100083E-10</v>
       </c>
       <c r="AF31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>22.993053551426648</v>
       </c>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH31" s="3">
+        <f t="shared" si="10"/>
+        <v>6448587.9214406693</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1944,15 +2065,15 @@
         <v>2.73874</v>
       </c>
       <c r="AB32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.1599999999999998E-4</v>
       </c>
       <c r="AC32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7599999999997671E-3</v>
       </c>
       <c r="AD32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5095402342.6048899</v>
       </c>
       <c r="AE32">
@@ -1960,11 +2081,15 @@
         <v>1.9625535586043171E-10</v>
       </c>
       <c r="AF32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>22.351604468629855</v>
       </c>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH32" s="3">
+        <f t="shared" si="10"/>
+        <v>4397279.6371158464</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>1</v>
       </c>
@@ -2021,15 +2146,15 @@
         <v>2.7366700000000002</v>
       </c>
       <c r="AB33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.9599999999999998E-4</v>
       </c>
       <c r="AC33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.6899999999999729E-3</v>
       </c>
       <c r="AD33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2981404648.3187323</v>
       </c>
       <c r="AE33">
@@ -2037,11 +2162,15 @@
         <v>3.3541237032816663E-10</v>
       </c>
       <c r="AF33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21.815660384905424</v>
       </c>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH33" s="3">
+        <f t="shared" si="10"/>
+        <v>3224293.9607203347</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -2116,15 +2245,15 @@
         <v>2.7353499999999999</v>
       </c>
       <c r="AB34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.84E-4</v>
       </c>
       <c r="AC34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.369999999999763E-3</v>
       </c>
       <c r="AD34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1873440562.6836548</v>
       </c>
       <c r="AE34">
@@ -2132,11 +2261,15 @@
         <v>5.3377727584136754E-10</v>
       </c>
       <c r="AF34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21.351042450412482</v>
       </c>
-    </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH34" s="3">
+        <f t="shared" si="10"/>
+        <v>2476303.0946128592</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2196,15 +2329,15 @@
         <v>2.7343500000000001</v>
       </c>
       <c r="AB35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.8E-4</v>
       </c>
       <c r="AC35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.3699999999998731E-3</v>
       </c>
       <c r="AD35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1205606972.6908014</v>
       </c>
       <c r="AE35">
@@ -2212,11 +2345,15 @@
         <v>8.2945771105495026E-10</v>
       </c>
       <c r="AF35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>20.910248988845435</v>
       </c>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH35" s="3">
+        <f t="shared" si="10"/>
+        <v>1909643.3475618931</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y36">
         <v>14</v>
       </c>
@@ -2228,15 +2365,15 @@
         <v>2.7335799999999999</v>
       </c>
       <c r="AB36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.8999999999999997E-4</v>
       </c>
       <c r="AC36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5999999999997137E-3</v>
       </c>
       <c r="AD36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>781858390.23678553</v>
       </c>
       <c r="AE36">
@@ -2244,11 +2381,15 @@
         <v>1.2790039890691079E-9</v>
       </c>
       <c r="AF36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>20.477184195457692</v>
       </c>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH36" s="3">
+        <f t="shared" si="10"/>
+        <v>1473315.342332511</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y37">
         <v>15</v>
       </c>
@@ -2260,15 +2401,15 @@
         <v>2.7329400000000001</v>
       </c>
       <c r="AB37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.0999999999999996E-4</v>
       </c>
       <c r="AC37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.9599999999999618E-3</v>
       </c>
       <c r="AD37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>502082282.50537735</v>
       </c>
       <c r="AE37">
@@ -2276,11 +2417,15 @@
         <v>1.9917054133239405E-9</v>
       </c>
       <c r="AF37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>20.034274573597592</v>
       </c>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH37" s="3">
+        <f t="shared" si="10"/>
+        <v>1110653.1042199936</v>
+      </c>
+    </row>
+    <row r="38" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -2288,7 +2433,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -2296,7 +2441,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -2336,8 +2481,11 @@
       <c r="AF40" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -2367,15 +2515,15 @@
         <v>2.7619600000000002</v>
       </c>
       <c r="AB41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="AC41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.0980000000000008E-2</v>
       </c>
       <c r="AD41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>292188134989.18567</v>
       </c>
       <c r="AE41">
@@ -2383,11 +2531,15 @@
         <v>3.4224524552888212E-12</v>
       </c>
       <c r="AF41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>26.400663729652077</v>
       </c>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH41" s="3">
+        <f>0.271/0.64 * $U$11 * AC41 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>17555118.963640861</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>1</v>
       </c>
@@ -2444,15 +2596,15 @@
         <v>2.7546900000000001</v>
       </c>
       <c r="AB42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.6999999999999999E-5</v>
       </c>
       <c r="AC42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.3709999999999898E-2</v>
       </c>
       <c r="AD42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>182209758952.08176</v>
       </c>
       <c r="AE42">
@@ -2460,11 +2612,15 @@
         <v>5.4881802475957615E-12</v>
       </c>
       <c r="AF42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25.928424382094651</v>
       </c>
-    </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH42" s="3">
+        <f t="shared" ref="AH42:AH55" si="11">0.271/0.64 * $U$11 * AC42 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>13435502.602579821</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -2539,15 +2695,15 @@
         <v>2.7551899999999998</v>
       </c>
       <c r="AB43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.6999999999999998E-5</v>
       </c>
       <c r="AC43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4209999999999621E-2</v>
       </c>
       <c r="AD43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>135767840156.62904</v>
       </c>
       <c r="AE43">
@@ -2555,11 +2711,15 @@
         <v>7.3655145345639034E-12</v>
       </c>
       <c r="AF43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25.634212206327398</v>
       </c>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH43" s="3">
+        <f t="shared" si="11"/>
+        <v>13718832.476105176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -2619,15 +2779,15 @@
         <v>2.7525200000000001</v>
       </c>
       <c r="AB44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.1999999999999997E-5</v>
       </c>
       <c r="AC44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1539999999999893E-2</v>
       </c>
       <c r="AD44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>85950062949.219452</v>
       </c>
       <c r="AE44">
@@ -2635,11 +2795,15 @@
         <v>1.1634662799384039E-11</v>
       </c>
       <c r="AF44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25.177032301168481</v>
       </c>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH44" s="3">
+        <f t="shared" si="11"/>
+        <v>12205850.951479087</v>
+      </c>
+    </row>
+    <row r="45" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y45">
         <v>5</v>
       </c>
@@ -2651,15 +2815,15 @@
         <v>2.7490000000000001</v>
       </c>
       <c r="AB45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.2000000000000002E-5</v>
       </c>
       <c r="AC45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.8019999999999925E-2</v>
       </c>
       <c r="AD45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>51930934041.277634</v>
       </c>
       <c r="AE45">
@@ -2667,11 +2831,15 @@
         <v>1.9256345345245351E-11</v>
       </c>
       <c r="AF45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24.673180481185803</v>
       </c>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH45" s="3">
+        <f t="shared" si="11"/>
+        <v>10211208.641859485</v>
+      </c>
+    </row>
+    <row r="46" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y46">
         <v>6</v>
       </c>
@@ -2683,15 +2851,15 @@
         <v>2.7454900000000002</v>
       </c>
       <c r="AB46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.02E-4</v>
       </c>
       <c r="AC46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.4510000000000023E-2</v>
       </c>
       <c r="AD46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>29516923141.827091</v>
       </c>
       <c r="AE46">
@@ -2699,11 +2867,15 @@
         <v>3.3878869934886453E-11</v>
       </c>
       <c r="AF46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24.108229601633496</v>
       </c>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH46" s="3">
+        <f t="shared" si="11"/>
+        <v>8222232.929710432</v>
+      </c>
+    </row>
+    <row r="47" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -2724,15 +2896,15 @@
         <v>2.7423299999999999</v>
       </c>
       <c r="AB47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4200000000000001E-4</v>
       </c>
       <c r="AC47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1349999999999749E-2</v>
       </c>
       <c r="AD47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>16584842857.908787</v>
       </c>
       <c r="AE47">
@@ -2740,11 +2912,15 @@
         <v>6.0296018995629588E-11</v>
       </c>
       <c r="AF47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>23.5317550343478</v>
       </c>
-    </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH47" s="3">
+        <f t="shared" si="11"/>
+        <v>6431588.12902903</v>
+      </c>
+    </row>
+    <row r="48" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -2762,15 +2938,15 @@
         <v>2.7395700000000001</v>
       </c>
       <c r="AB48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.92E-4</v>
       </c>
       <c r="AC48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.5899999999998755E-3</v>
       </c>
       <c r="AD48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9283158783.5995483</v>
       </c>
       <c r="AE48">
@@ -2778,11 +2954,15 @@
         <v>1.0772195362710899E-10</v>
       </c>
       <c r="AF48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>22.951467711990038</v>
       </c>
-    </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH48" s="3">
+        <f t="shared" si="11"/>
+        <v>4867607.227168262</v>
+      </c>
+    </row>
+    <row r="49" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -2800,15 +2980,15 @@
         <v>2.7378200000000001</v>
       </c>
       <c r="AB49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.52E-4</v>
       </c>
       <c r="AC49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.8399999999999572E-3</v>
       </c>
       <c r="AD49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5631957964.838089</v>
       </c>
       <c r="AE49">
@@ -2816,11 +2996,15 @@
         <v>1.7755814341003317E-10</v>
       </c>
       <c r="AF49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>22.451722992144699</v>
       </c>
-    </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH49" s="3">
+        <f t="shared" si="11"/>
+        <v>3875952.6698290082</v>
+      </c>
+    </row>
+    <row r="50" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -2838,15 +3022,15 @@
         <v>2.7361800000000001</v>
       </c>
       <c r="AB50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2400000000000001E-4</v>
       </c>
       <c r="AC50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.1999999999998714E-3</v>
       </c>
       <c r="AD50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3330137588.0458527</v>
       </c>
       <c r="AE50">
@@ -2854,11 +3038,15 @@
         <v>3.0028789308576493E-10</v>
       </c>
       <c r="AF50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21.926279457816698</v>
       </c>
-    </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH50" s="3">
+        <f t="shared" si="11"/>
+        <v>2946630.6846652734</v>
+      </c>
+    </row>
+    <row r="51" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>1</v>
       </c>
@@ -2915,15 +3103,15 @@
         <v>2.7351999999999999</v>
       </c>
       <c r="AB51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.0400000000000001E-4</v>
       </c>
       <c r="AC51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.2199999999996685E-3</v>
       </c>
       <c r="AD51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2167379341.8617129</v>
       </c>
       <c r="AE51">
@@ -2931,11 +3119,15 @@
         <v>4.6138669898967961E-10</v>
       </c>
       <c r="AF51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21.496784598108359</v>
       </c>
-    </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH51" s="3">
+        <f t="shared" si="11"/>
+        <v>2391304.1325551514</v>
+      </c>
+    </row>
+    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -3010,15 +3202,15 @@
         <v>2.7343000000000002</v>
       </c>
       <c r="AB52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.8999999999999998E-4</v>
       </c>
       <c r="AC52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.3199999999999896E-3</v>
       </c>
       <c r="AD52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1405872213.7791362</v>
       </c>
       <c r="AE52">
@@ -3026,11 +3218,15 @@
         <v>7.1130220101007055E-10</v>
       </c>
       <c r="AF52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21.063923739845389</v>
       </c>
-    </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH52" s="3">
+        <f t="shared" si="11"/>
+        <v>1881310.3602094075</v>
+      </c>
+    </row>
+    <row r="53" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -3090,15 +3286,15 @@
         <v>2.7336200000000002</v>
       </c>
       <c r="AB53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.9000000000000003E-4</v>
       </c>
       <c r="AC53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.6399999999999757E-3</v>
       </c>
       <c r="AD53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>928444096.25519705</v>
       </c>
       <c r="AE53">
@@ -3106,11 +3302,15 @@
         <v>1.0770707725251502E-9</v>
       </c>
       <c r="AF53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>20.649020728280121</v>
       </c>
-    </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH53" s="3">
+        <f t="shared" si="11"/>
+        <v>1495981.7322147004</v>
+      </c>
+    </row>
+    <row r="54" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y54">
         <v>14</v>
       </c>
@@ -3122,15 +3322,15 @@
         <v>2.7330399999999999</v>
       </c>
       <c r="AB54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="AC54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.0599999999997287E-3</v>
       </c>
       <c r="AD54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>610622810.92447412</v>
       </c>
       <c r="AE54">
@@ -3138,11 +3338,15 @@
         <v>1.6376721965005114E-9</v>
       </c>
       <c r="AF54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>20.229989995779622</v>
       </c>
-    </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH54" s="3">
+        <f t="shared" si="11"/>
+        <v>1167319.0789249642</v>
+      </c>
+    </row>
+    <row r="55" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y55">
         <v>15</v>
       </c>
@@ -3154,15 +3358,15 @@
         <v>2.7325699999999999</v>
       </c>
       <c r="AB55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.1999999999999998E-4</v>
       </c>
       <c r="AC55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.5899999999997583E-3</v>
       </c>
       <c r="AD55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>402334352.68702698</v>
       </c>
       <c r="AE55">
@@ -3170,11 +3374,15 @@
         <v>2.4854949454885174E-9</v>
       </c>
       <c r="AF55">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>19.812794023995359</v>
       </c>
-    </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH55" s="3">
+        <f t="shared" si="11"/>
+        <v>900988.99781099788</v>
+      </c>
+    </row>
+    <row r="56" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -3192,15 +3400,15 @@
         <v>2.7322000000000002</v>
       </c>
       <c r="AB56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.5E-4</v>
       </c>
       <c r="AC56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.2199999999999989E-3</v>
       </c>
       <c r="AD56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>266464936.3973271</v>
       </c>
       <c r="AE56">
@@ -3208,11 +3416,11 @@
         <v>3.7528389795680108E-9</v>
       </c>
       <c r="AF56">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>19.400753222172249</v>
       </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -3220,7 +3428,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -3228,7 +3436,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -3268,8 +3476,11 @@
       <c r="AF59" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>1</v>
       </c>
@@ -3338,15 +3549,15 @@
         <v>2.7751399999999999</v>
       </c>
       <c r="AB60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.16E-4</v>
       </c>
       <c r="AC60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.4159999999999755E-2</v>
       </c>
       <c r="AD60">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>78990510258.20105</v>
       </c>
       <c r="AE60">
@@ -3354,11 +3565,15 @@
         <v>1.265974857905386E-11</v>
       </c>
       <c r="AF60">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25.09259355888414</v>
       </c>
-    </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH60" s="3">
+        <f>0.271/0.64 * $U$11 * AC60 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>25023694.429773264</v>
+      </c>
+    </row>
+    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -3433,15 +3648,15 @@
         <v>2.77413</v>
       </c>
       <c r="AB61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.22E-4</v>
       </c>
       <c r="AC61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.31499999999998E-2</v>
       </c>
       <c r="AD61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>73387959589.27298</v>
       </c>
       <c r="AE61">
@@ -3449,11 +3664,15 @@
         <v>1.3626213422428612E-11</v>
       </c>
       <c r="AF61">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25.019025720817844</v>
       </c>
-    </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH61" s="3">
+        <f t="shared" ref="AH61:AH74" si="12">0.271/0.64 * $U$11 * AC61 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>24451368.085251752</v>
+      </c>
+    </row>
+    <row r="62" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -3513,15 +3732,15 @@
         <v>2.7735099999999999</v>
       </c>
       <c r="AB62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3200000000000001E-4</v>
       </c>
       <c r="AC62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.2529999999999735E-2</v>
       </c>
       <c r="AD62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>66853676463.793755</v>
       </c>
       <c r="AE62">
@@ -3529,11 +3748,15 @@
         <v>1.495804049821515E-11</v>
       </c>
       <c r="AF62">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24.925772134700836</v>
       </c>
-    </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH62" s="3">
+        <f t="shared" si="12"/>
+        <v>24100039.042080078</v>
+      </c>
+    </row>
+    <row r="63" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y63">
         <v>4</v>
       </c>
@@ -3545,15 +3768,15 @@
         <v>2.7711100000000002</v>
       </c>
       <c r="AB63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4799999999999999E-4</v>
       </c>
       <c r="AC63">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.0129999999999999E-2</v>
       </c>
       <c r="AD63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>56261497578.331345</v>
       </c>
       <c r="AE63">
@@ -3561,11 +3784,15 @@
         <v>1.7774144717845936E-11</v>
       </c>
       <c r="AF63">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24.753276258536378</v>
       </c>
-    </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH63" s="3">
+        <f t="shared" si="12"/>
+        <v>22740055.649157763</v>
+      </c>
+    </row>
+    <row r="64" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y64">
         <v>5</v>
       </c>
@@ -3577,15 +3804,15 @@
         <v>2.7686700000000002</v>
       </c>
       <c r="AB64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6799999999999999E-4</v>
       </c>
       <c r="AC64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.7690000000000001E-2</v>
       </c>
       <c r="AD64">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>46550108704.9888</v>
       </c>
       <c r="AE64">
@@ -3593,11 +3820,15 @@
         <v>2.1482226955419107E-11</v>
       </c>
       <c r="AF64">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24.563795175897454</v>
       </c>
-    </row>
-    <row r="65" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH64" s="3">
+        <f t="shared" si="12"/>
+        <v>21357405.866353251</v>
+      </c>
+    </row>
+    <row r="65" spans="21:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y65">
         <v>6</v>
       </c>
@@ -3609,15 +3840,15 @@
         <v>2.7652600000000001</v>
       </c>
       <c r="AB65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.9799999999999999E-4</v>
       </c>
       <c r="AC65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.4279999999999866E-2</v>
       </c>
       <c r="AD65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35923568135.102371</v>
       </c>
       <c r="AE65">
@@ -3625,11 +3856,15 @@
         <v>2.7836878459265842E-11</v>
       </c>
       <c r="AF65">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24.304659411056708</v>
       </c>
-    </row>
-    <row r="66" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH65" s="3">
+        <f t="shared" si="12"/>
+        <v>19425096.128909171</v>
+      </c>
+    </row>
+    <row r="66" spans="21:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y66">
         <v>7</v>
       </c>
@@ -3641,15 +3876,15 @@
         <v>2.7614000000000001</v>
       </c>
       <c r="AB66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.4000000000000001E-4</v>
       </c>
       <c r="AC66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.0419999999999892E-2</v>
       </c>
       <c r="AD66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26299761601.592667</v>
       </c>
       <c r="AE66">
@@ -3657,11 +3892,15 @@
         <v>3.8023158352106193E-11</v>
       </c>
       <c r="AF66">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>23.992825711510822</v>
       </c>
-    </row>
-    <row r="67" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH66" s="3">
+        <f t="shared" si="12"/>
+        <v>17237789.505292218</v>
+      </c>
+    </row>
+    <row r="67" spans="21:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y67">
         <v>8</v>
       </c>
@@ -3673,15 +3912,15 @@
         <v>2.7567900000000001</v>
       </c>
       <c r="AB67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.92E-4</v>
       </c>
       <c r="AC67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5809999999999889E-2</v>
       </c>
       <c r="AD67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>18340408174.248367</v>
       </c>
       <c r="AE67">
@@ -3689,11 +3928,15 @@
         <v>5.4524413551716516E-11</v>
       </c>
       <c r="AF67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>23.632372559483905</v>
       </c>
-    </row>
-    <row r="68" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH67" s="3">
+        <f t="shared" si="12"/>
+        <v>14625488.071386974</v>
+      </c>
+    </row>
+    <row r="68" spans="21:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y68">
         <v>9</v>
       </c>
@@ -3705,15 +3948,15 @@
         <v>2.7533300000000001</v>
       </c>
       <c r="AB68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.5199999999999999E-4</v>
       </c>
       <c r="AC68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.234999999999987E-2</v>
       </c>
       <c r="AD68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13174638510.749393</v>
       </c>
       <c r="AE68">
@@ -3721,11 +3964,15 @@
         <v>7.590341087416435E-11</v>
       </c>
       <c r="AF68">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>23.301559493483143</v>
       </c>
-    </row>
-    <row r="69" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH68" s="3">
+        <f t="shared" si="12"/>
+        <v>12664845.346590409</v>
+      </c>
+    </row>
+    <row r="69" spans="21:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y69">
         <v>10</v>
       </c>
@@ -3737,15 +3984,15 @@
         <v>2.7495500000000002</v>
       </c>
       <c r="AB69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.2400000000000001E-4</v>
       </c>
       <c r="AC69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.8569999999999975E-2</v>
       </c>
       <c r="AD69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9087614397.3349895</v>
       </c>
       <c r="AE69">
@@ -3753,11 +4000,15 @@
         <v>1.1003988024549737E-10</v>
       </c>
       <c r="AF69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>22.930178268154325</v>
       </c>
-    </row>
-    <row r="70" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH69" s="3">
+        <f t="shared" si="12"/>
+        <v>10522871.502737582</v>
+      </c>
+    </row>
+    <row r="70" spans="21:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y70">
         <v>11</v>
       </c>
@@ -3769,27 +4020,31 @@
         <v>2.7464900000000001</v>
       </c>
       <c r="AB70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="AC70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.5509999999999913E-2</v>
       </c>
       <c r="AD70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6436438697.289176</v>
       </c>
       <c r="AE70">
-        <f t="shared" ref="AE70:AE128" si="9">1/AD70</f>
+        <f t="shared" ref="AE70:AE128" si="13">1/AD70</f>
         <v>1.5536541976561795E-10</v>
       </c>
       <c r="AF70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>22.585241226787918</v>
       </c>
-    </row>
-    <row r="71" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH70" s="3">
+        <f t="shared" si="12"/>
+        <v>8788892.6767614</v>
+      </c>
+    </row>
+    <row r="71" spans="21:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y71">
         <v>12</v>
       </c>
@@ -3801,27 +4056,31 @@
         <v>2.74316</v>
       </c>
       <c r="AB71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.9000000000000003E-4</v>
       </c>
       <c r="AC71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.2179999999999858E-2</v>
       </c>
       <c r="AD71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4283503444.0864658</v>
       </c>
       <c r="AE71">
+        <f t="shared" si="13"/>
+        <v>2.3345376350298882E-10</v>
+      </c>
+      <c r="AF71">
         <f t="shared" si="9"/>
-        <v>2.3345376350298882E-10</v>
-      </c>
-      <c r="AF71">
-        <f t="shared" si="8"/>
         <v>22.178037073403644</v>
       </c>
-    </row>
-    <row r="72" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH71" s="3">
+        <f t="shared" si="12"/>
+        <v>6901915.7190814419</v>
+      </c>
+    </row>
+    <row r="72" spans="21:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y72">
         <v>13</v>
       </c>
@@ -3833,27 +4092,31 @@
         <v>2.7406700000000002</v>
       </c>
       <c r="AB72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.8999999999999997E-4</v>
       </c>
       <c r="AC72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.6899999999999764E-3</v>
       </c>
       <c r="AD72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2913926077.4597187</v>
       </c>
       <c r="AE72">
+        <f t="shared" si="13"/>
+        <v>3.4317960491014678E-10</v>
+      </c>
+      <c r="AF72">
         <f t="shared" si="9"/>
-        <v>3.4317960491014678E-10</v>
-      </c>
-      <c r="AF72">
-        <f t="shared" si="8"/>
         <v>21.792767176333037</v>
       </c>
-    </row>
-    <row r="73" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH72" s="3">
+        <f t="shared" si="12"/>
+        <v>5490932.9489244483</v>
+      </c>
+    </row>
+    <row r="73" spans="21:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y73">
         <v>14</v>
       </c>
@@ -3865,27 +4128,31 @@
         <v>2.7385700000000002</v>
       </c>
       <c r="AB73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="AC73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.5899999999999856E-3</v>
       </c>
       <c r="AD73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1968591622.8411114</v>
       </c>
       <c r="AE73">
+        <f t="shared" si="13"/>
+        <v>5.079773724510621E-10</v>
+      </c>
+      <c r="AF73">
         <f t="shared" si="9"/>
-        <v>5.079773724510621E-10</v>
-      </c>
-      <c r="AF73">
-        <f t="shared" si="8"/>
         <v>21.400584211761277</v>
       </c>
-    </row>
-    <row r="74" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH73" s="3">
+        <f t="shared" si="12"/>
+        <v>4300947.4801172959</v>
+      </c>
+    </row>
+    <row r="74" spans="21:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Y74">
         <v>15</v>
       </c>
@@ -3897,27 +4164,31 @@
         <v>2.7365400000000002</v>
       </c>
       <c r="AB74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.2000000000000003E-4</v>
       </c>
       <c r="AC74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.5600000000000094E-3</v>
       </c>
       <c r="AD74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1253980572.0337536</v>
       </c>
       <c r="AE74">
+        <f t="shared" si="13"/>
+        <v>7.9746052076242436E-10</v>
+      </c>
+      <c r="AF74">
         <f t="shared" si="9"/>
-        <v>7.9746052076242436E-10</v>
-      </c>
-      <c r="AF74">
-        <f t="shared" si="8"/>
         <v>20.949588786241076</v>
       </c>
-    </row>
-    <row r="77" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH74" s="3">
+        <f t="shared" si="12"/>
+        <v>3150628.1936037214</v>
+      </c>
+    </row>
+    <row r="77" spans="21:34" x14ac:dyDescent="0.3">
       <c r="U77" t="s">
         <v>1</v>
       </c>
@@ -3951,8 +4222,11 @@
       <c r="AF77" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="78" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="21:34" x14ac:dyDescent="0.3">
       <c r="U78" s="1">
         <v>200</v>
       </c>
@@ -3976,27 +4250,31 @@
         <v>2.7715999999999998</v>
       </c>
       <c r="AB78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="AC78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.0619999999999656E-2</v>
       </c>
       <c r="AD78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>42141866519.001541</v>
       </c>
       <c r="AE78">
+        <f t="shared" si="13"/>
+        <v>2.3729371349726651E-11</v>
+      </c>
+      <c r="AF78">
         <f t="shared" si="9"/>
-        <v>2.3729371349726651E-11</v>
-      </c>
-      <c r="AF78">
-        <f t="shared" si="8"/>
         <v>24.464307537625864</v>
       </c>
-    </row>
-    <row r="79" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH78" s="3">
+        <f>0.271/0.64 * $U$11 * AC78 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>23017718.925212566</v>
+      </c>
+    </row>
+    <row r="79" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y79">
         <v>2</v>
       </c>
@@ -4008,27 +4286,31 @@
         <v>2.7696999999999998</v>
       </c>
       <c r="AB79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.12E-4</v>
       </c>
       <c r="AC79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.8719999999999644E-2</v>
       </c>
       <c r="AD79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>37896869086.139793</v>
       </c>
       <c r="AE79">
+        <f t="shared" si="13"/>
+        <v>2.638740413428335E-11</v>
+      </c>
+      <c r="AF79">
         <f t="shared" si="9"/>
-        <v>2.638740413428335E-11</v>
-      </c>
-      <c r="AF79">
-        <f t="shared" si="8"/>
         <v>24.358134335758024</v>
       </c>
-    </row>
-    <row r="80" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH79" s="3">
+        <f t="shared" ref="AH79:AH92" si="14">0.271/0.64 * $U$11 * AC79 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>21941065.405815609</v>
+      </c>
+    </row>
+    <row r="80" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y80">
         <v>3</v>
       </c>
@@ -4040,27 +4322,31 @@
         <v>2.7667999999999999</v>
       </c>
       <c r="AB80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.32E-4</v>
       </c>
       <c r="AC80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.5819999999999741E-2</v>
       </c>
       <c r="AD80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>32036232760.968712</v>
       </c>
       <c r="AE80">
+        <f t="shared" si="13"/>
+        <v>3.1214656462926823E-11</v>
+      </c>
+      <c r="AF80">
         <f t="shared" si="9"/>
-        <v>3.1214656462926823E-11</v>
-      </c>
-      <c r="AF80">
-        <f t="shared" si="8"/>
         <v>24.190133372987919</v>
       </c>
-    </row>
-    <row r="81" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH80" s="3">
+        <f t="shared" si="14"/>
+        <v>20297752.139367681</v>
+      </c>
+    </row>
+    <row r="81" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y81">
         <v>4</v>
       </c>
@@ -4072,27 +4358,31 @@
         <v>2.76491</v>
       </c>
       <c r="AB81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.6400000000000002E-4</v>
       </c>
       <c r="AC81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.3929999999999794E-2</v>
       </c>
       <c r="AD81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26667590435.181313</v>
       </c>
       <c r="AE81">
+        <f t="shared" si="13"/>
+        <v>3.7498700995525508E-11</v>
+      </c>
+      <c r="AF81">
         <f t="shared" si="9"/>
-        <v>3.7498700995525508E-11</v>
-      </c>
-      <c r="AF81">
-        <f t="shared" si="8"/>
         <v>24.006714823671487</v>
       </c>
-    </row>
-    <row r="82" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH81" s="3">
+        <f t="shared" si="14"/>
+        <v>19226765.217441272</v>
+      </c>
+    </row>
+    <row r="82" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y82">
         <v>5</v>
       </c>
@@ -4104,27 +4394,31 @@
         <v>2.7613699999999999</v>
       </c>
       <c r="AB82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.1199999999999999E-4</v>
       </c>
       <c r="AC82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.0389999999999695E-2</v>
       </c>
       <c r="AD82">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>20210634579.28479</v>
       </c>
       <c r="AE82">
+        <f t="shared" si="13"/>
+        <v>4.9478901618703542E-11</v>
+      </c>
+      <c r="AF82">
         <f t="shared" si="9"/>
-        <v>4.9478901618703542E-11</v>
-      </c>
-      <c r="AF82">
-        <f t="shared" si="8"/>
         <v>23.729474767140879</v>
       </c>
-    </row>
-    <row r="83" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH82" s="3">
+        <f t="shared" si="14"/>
+        <v>17220789.712880574</v>
+      </c>
+    </row>
+    <row r="83" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y83">
         <v>6</v>
       </c>
@@ -4136,27 +4430,31 @@
         <v>2.7570100000000002</v>
       </c>
       <c r="AB83">
-        <f t="shared" ref="AB83:AB128" si="10">Z83/1000000</f>
+        <f t="shared" ref="AB83:AB128" si="15">Z83/1000000</f>
         <v>3.8000000000000002E-4</v>
       </c>
       <c r="AC83">
-        <f t="shared" ref="AC83:AC128" si="11">AA83-$X$5</f>
+        <f t="shared" ref="AC83:AC128" si="16">AA83-$X$5</f>
         <v>2.6029999999999998E-2</v>
       </c>
       <c r="AD83">
-        <f t="shared" ref="AD83:AD128" si="12">(0.271*0.04^2*AC83*1000000000*8*PI()^2*8.854*0.000000000001*9.107*1E-31)/(0.64*0.009^2*(1.602*0.0000000000000000001)^2*(Z83/1000000))</f>
+        <f t="shared" ref="AD83:AD128" si="17">(0.271*0.04^2*AC83*1000000000*8*PI()^2*8.854*0.000000000001*9.107*1E-31)/(0.64*0.009^2*(1.602*0.0000000000000000001)^2*(Z83/1000000))</f>
         <v>14213283390.209896</v>
       </c>
       <c r="AE83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>7.0356720016488214E-11</v>
       </c>
       <c r="AF83">
-        <f t="shared" ref="AF83:AF128" si="13">LN(AD83)</f>
+        <f t="shared" ref="AF83:AF128" si="18">LN(AD83)</f>
         <v>23.377442814307713</v>
       </c>
-    </row>
-    <row r="84" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH83" s="3">
+        <f t="shared" si="14"/>
+        <v>14750153.215738263</v>
+      </c>
+    </row>
+    <row r="84" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y84">
         <v>7</v>
       </c>
@@ -4168,27 +4466,31 @@
         <v>2.7521599999999999</v>
       </c>
       <c r="AB84">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>4.7600000000000002E-4</v>
       </c>
       <c r="AC84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.1179999999999755E-2</v>
       </c>
       <c r="AD84">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>9232575053.8134747</v>
       </c>
       <c r="AE84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.0831214413869881E-10</v>
       </c>
       <c r="AF84">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>22.946003833963498</v>
       </c>
-    </row>
-    <row r="85" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH84" s="3">
+        <f t="shared" si="14"/>
+        <v>12001853.44254064</v>
+      </c>
+    </row>
+    <row r="85" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y85">
         <v>8</v>
       </c>
@@ -4200,27 +4502,31 @@
         <v>2.7478699999999998</v>
       </c>
       <c r="AB85">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="AC85">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.6889999999999628E-2</v>
       </c>
       <c r="AD85">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>5840933247.217515</v>
       </c>
       <c r="AE85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.712055176244955E-10</v>
       </c>
       <c r="AF85">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>22.48815642362521</v>
       </c>
-    </row>
-    <row r="86" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH85" s="3">
+        <f t="shared" si="14"/>
+        <v>9570883.1276916545</v>
+      </c>
+    </row>
+    <row r="86" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y86">
         <v>9</v>
       </c>
@@ -4232,27 +4538,31 @@
         <v>2.7444999999999999</v>
       </c>
       <c r="AB86">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>7.2000000000000005E-4</v>
       </c>
       <c r="AC86">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.3519999999999754E-2</v>
       </c>
       <c r="AD86">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>3896260978.0136719</v>
       </c>
       <c r="AE86">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.5665631887672054E-10</v>
       </c>
       <c r="AF86">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>22.083283206626369</v>
       </c>
-    </row>
-    <row r="87" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH86" s="3">
+        <f t="shared" si="14"/>
+        <v>7661239.7801297624</v>
+      </c>
+    </row>
+    <row r="87" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y87">
         <v>10</v>
       </c>
@@ -4264,27 +4574,31 @@
         <v>2.7416999999999998</v>
       </c>
       <c r="AB87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.5999999999999998E-4</v>
       </c>
       <c r="AC87">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.0719999999999619E-2</v>
       </c>
       <c r="AD87">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>2586426717.7566571</v>
       </c>
       <c r="AE87">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>3.8663380374733839E-10</v>
       </c>
       <c r="AF87">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>21.673543114416734</v>
       </c>
-    </row>
-    <row r="88" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH87" s="3">
+        <f t="shared" si="14"/>
+        <v>6074592.4883868061</v>
+      </c>
+    </row>
+    <row r="88" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y88">
         <v>11</v>
       </c>
@@ -4296,27 +4610,31 @@
         <v>2.7394699999999998</v>
       </c>
       <c r="AB88">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.0499999999999999E-3</v>
       </c>
       <c r="AC88">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>8.4899999999996645E-3</v>
       </c>
       <c r="AD88">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>1677730635.8411851</v>
       </c>
       <c r="AE88">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>5.9604323759553764E-10</v>
       </c>
       <c r="AF88">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>21.240707905193318</v>
       </c>
-    </row>
-    <row r="89" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH88" s="3">
+        <f t="shared" si="14"/>
+        <v>4810941.252463039</v>
+      </c>
+    </row>
+    <row r="89" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y89">
         <v>12</v>
       </c>
@@ -4328,27 +4646,31 @@
         <v>2.7374800000000001</v>
       </c>
       <c r="AB89">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.24E-3</v>
       </c>
       <c r="AC89">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>6.4999999999999503E-3</v>
       </c>
       <c r="AD89">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>1087665905.7730587</v>
       </c>
       <c r="AE89">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>9.193999689539316E-10</v>
       </c>
       <c r="AF89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>20.807299866324168</v>
       </c>
-    </row>
-    <row r="90" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH89" s="3">
+        <f t="shared" si="14"/>
+        <v>3683288.3558316547</v>
+      </c>
+    </row>
+    <row r="90" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y90">
         <v>13</v>
       </c>
@@ -4360,27 +4682,31 @@
         <v>2.7359100000000001</v>
       </c>
       <c r="AB90">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.4E-3</v>
       </c>
       <c r="AC90">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>4.9299999999998789E-3</v>
       </c>
       <c r="AD90">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>730672441.22766495</v>
       </c>
       <c r="AE90">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.3686023224303011E-9</v>
       </c>
       <c r="AF90">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>20.409475820472892</v>
       </c>
-    </row>
-    <row r="91" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH90" s="3">
+        <f t="shared" si="14"/>
+        <v>2793632.5529615004</v>
+      </c>
+    </row>
+    <row r="91" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y91">
         <v>14</v>
       </c>
@@ -4392,27 +4718,31 @@
         <v>2.7353999999999998</v>
       </c>
       <c r="AB91">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.5E-3</v>
       </c>
       <c r="AC91">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>4.4199999999996464E-3</v>
       </c>
       <c r="AD91">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>611413261.16518462</v>
       </c>
       <c r="AE91">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.6355549732341044E-9</v>
       </c>
       <c r="AF91">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>20.231283657020896</v>
       </c>
-    </row>
-    <row r="92" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH91" s="3">
+        <f t="shared" si="14"/>
+        <v>2504636.081965344</v>
+      </c>
+    </row>
+    <row r="92" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y92">
         <v>15</v>
       </c>
@@ -4424,27 +4754,31 @@
         <v>2.7348300000000001</v>
       </c>
       <c r="AB92">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="AC92">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>3.8499999999999091E-3</v>
       </c>
       <c r="AD92">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>499280484.05389428</v>
       </c>
       <c r="AE92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.0028822113785165E-9</v>
       </c>
       <c r="AF92">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>20.028678588093467</v>
       </c>
-    </row>
-    <row r="95" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH92" s="3">
+        <f t="shared" si="14"/>
+        <v>2181640.0261464068</v>
+      </c>
+    </row>
+    <row r="95" spans="21:34" x14ac:dyDescent="0.3">
       <c r="U95" t="s">
         <v>1</v>
       </c>
@@ -4478,8 +4812,11 @@
       <c r="AF95" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="96" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="21:34" x14ac:dyDescent="0.3">
       <c r="U96" s="1">
         <v>450</v>
       </c>
@@ -4503,27 +4840,31 @@
         <v>2.7692899999999998</v>
       </c>
       <c r="AB96">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>2.7999999999999998E-4</v>
       </c>
       <c r="AC96">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>3.8309999999999622E-2</v>
       </c>
       <c r="AD96">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>28389514425.387684</v>
       </c>
       <c r="AE96">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>3.5224272772546515E-11</v>
       </c>
       <c r="AF96">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>24.069285703564969</v>
       </c>
-    </row>
-    <row r="97" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH96" s="3">
+        <f>0.271/0.64 * $U$11 * AC96 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>21708734.909524668</v>
+      </c>
+    </row>
+    <row r="97" spans="21:34" x14ac:dyDescent="0.3">
       <c r="U97" t="s">
         <v>7</v>
       </c>
@@ -4538,27 +4879,31 @@
         <v>2.7662800000000001</v>
       </c>
       <c r="AB97">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="AC97">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>3.5299999999999887E-2</v>
       </c>
       <c r="AD97">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>24415031808.973614</v>
       </c>
       <c r="AE97">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>4.0958373833961398E-11</v>
       </c>
       <c r="AF97">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>23.918464837304715</v>
       </c>
-    </row>
-    <row r="98" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH97" s="3">
+        <f t="shared" ref="AH97:AH110" si="19">0.271/0.64 * $U$11 * AC97 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>20003089.070901226</v>
+      </c>
+    </row>
+    <row r="98" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y98">
         <v>3</v>
       </c>
@@ -4570,27 +4915,31 @@
         <v>2.7647300000000001</v>
       </c>
       <c r="AB98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>3.3E-4</v>
       </c>
       <c r="AC98">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>3.3749999999999947E-2</v>
       </c>
       <c r="AD98">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>21220894245.50246</v>
       </c>
       <c r="AE98">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>4.7123367584376859E-11</v>
       </c>
       <c r="AF98">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>23.778252110879681</v>
       </c>
-    </row>
-    <row r="99" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH98" s="3">
+        <f t="shared" si="19"/>
+        <v>19124766.462972172</v>
+      </c>
+    </row>
+    <row r="99" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y99">
         <v>4</v>
       </c>
@@ -4602,27 +4951,31 @@
         <v>2.7596799999999999</v>
       </c>
       <c r="AB99">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>3.8000000000000002E-4</v>
       </c>
       <c r="AC99">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.8699999999999726E-2</v>
       </c>
       <c r="AD99">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>15671196054.514793</v>
       </c>
       <c r="AE99">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>6.3811338746662226E-11</v>
       </c>
       <c r="AF99">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>23.475090218066804</v>
       </c>
-    </row>
-    <row r="100" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH99" s="3">
+        <f t="shared" si="19"/>
+        <v>16263134.740364349</v>
+      </c>
+    </row>
+    <row r="100" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y100">
         <v>5</v>
       </c>
@@ -4634,27 +4987,31 @@
         <v>2.7560899999999999</v>
       </c>
       <c r="AB100">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>4.4000000000000002E-4</v>
       </c>
       <c r="AC100">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.5109999999999744E-2</v>
       </c>
       <c r="AD100">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>11841258988.990278</v>
       </c>
       <c r="AE100">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>8.4450479541894681E-11</v>
       </c>
       <c r="AF100">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>23.194855794278848</v>
       </c>
-    </row>
-    <row r="101" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH100" s="3">
+        <f t="shared" si="19"/>
+        <v>14228826.248451173</v>
+      </c>
+    </row>
+    <row r="101" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y101">
         <v>6</v>
       </c>
@@ -4666,27 +5023,31 @@
         <v>2.75359</v>
       </c>
       <c r="AB101">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>5.1000000000000004E-4</v>
       </c>
       <c r="AC101">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.2609999999999797E-2</v>
       </c>
       <c r="AD101">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>9198864675.9021854</v>
       </c>
       <c r="AE101">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.0870906739389818E-10</v>
       </c>
       <c r="AF101">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>22.942345908593168</v>
       </c>
-    </row>
-    <row r="102" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH101" s="3">
+        <f t="shared" si="19"/>
+        <v>12812176.880823633</v>
+      </c>
+    </row>
+    <row r="102" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y102">
         <v>7</v>
       </c>
@@ -4698,27 +5059,31 @@
         <v>2.7495799999999999</v>
       </c>
       <c r="AB102">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>6.2E-4</v>
       </c>
       <c r="AC102">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.8599999999999728E-2</v>
       </c>
       <c r="AD102">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>6224795645.3473082</v>
       </c>
       <c r="AE102">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.6064784403765045E-10</v>
       </c>
       <c r="AF102">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>22.551806450701672</v>
       </c>
-    </row>
-    <row r="103" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH102" s="3">
+        <f t="shared" si="19"/>
+        <v>10539871.295148969</v>
+      </c>
+    </row>
+    <row r="103" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y103">
         <v>8</v>
       </c>
@@ -4730,27 +5095,31 @@
         <v>2.74593</v>
       </c>
       <c r="AB103">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>7.6999999999999996E-4</v>
       </c>
       <c r="AC103">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.4949999999999797E-2</v>
       </c>
       <c r="AD103">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>4028601510.7334356</v>
       </c>
       <c r="AE103">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.4822509680733918E-10</v>
       </c>
       <c r="AF103">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>22.11668513301062</v>
       </c>
-    </row>
-    <row r="104" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH103" s="3">
+        <f t="shared" si="19"/>
+        <v>8471563.2184127569</v>
+      </c>
+    </row>
+    <row r="104" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y104">
         <v>9</v>
       </c>
@@ -4762,27 +5131,31 @@
         <v>2.7421199999999999</v>
       </c>
       <c r="AB104">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>9.7000000000000005E-4</v>
       </c>
       <c r="AC104">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.1139999999999706E-2</v>
       </c>
       <c r="AD104">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>2382963006.5006251</v>
       </c>
       <c r="AE104">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>4.1964562490984589E-10</v>
       </c>
       <c r="AF104">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>21.591610511023351</v>
       </c>
-    </row>
-    <row r="105" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH104" s="3">
+        <f t="shared" si="19"/>
+        <v>6312589.5821482884</v>
+      </c>
+    </row>
+    <row r="105" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y105">
         <v>10</v>
       </c>
@@ -4794,27 +5167,31 @@
         <v>2.7396400000000001</v>
       </c>
       <c r="AB105">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.2199999999999999E-3</v>
       </c>
       <c r="AC105">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>8.65999999999989E-3</v>
       </c>
       <c r="AD105">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>1472861483.2980278</v>
       </c>
       <c r="AE105">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>6.7895047249168498E-10</v>
       </c>
       <c r="AF105">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>21.110472932868699</v>
       </c>
-    </row>
-    <row r="106" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH105" s="3">
+        <f t="shared" si="19"/>
+        <v>4907273.4094618419</v>
+      </c>
+    </row>
+    <row r="106" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y106">
         <v>11</v>
       </c>
@@ -4826,27 +5203,31 @@
         <v>2.7378999999999998</v>
       </c>
       <c r="AB106">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.4599999999999999E-3</v>
       </c>
       <c r="AC106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>6.9199999999995931E-3</v>
       </c>
       <c r="AD106">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>983460864.51601553</v>
       </c>
       <c r="AE106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.0168172787354622E-9</v>
       </c>
       <c r="AF106">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>20.706588402948807</v>
       </c>
-    </row>
-    <row r="107" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH106" s="3">
+        <f t="shared" si="19"/>
+        <v>3921285.4495928842</v>
+      </c>
+    </row>
+    <row r="107" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y107">
         <v>12</v>
       </c>
@@ -4858,27 +5239,31 @@
         <v>2.73672</v>
       </c>
       <c r="AB107">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.7600000000000001E-3</v>
       </c>
       <c r="AC107">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>5.7399999999998563E-3</v>
       </c>
       <c r="AD107">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>676710738.7176739</v>
       </c>
       <c r="AE107">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.4777362657122004E-9</v>
       </c>
       <c r="AF107">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>20.332754470320921</v>
       </c>
-    </row>
-    <row r="108" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH107" s="3">
+        <f t="shared" si="19"/>
+        <v>3252626.94807282</v>
+      </c>
+    </row>
+    <row r="108" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y108">
         <v>13</v>
       </c>
@@ -4890,27 +5275,31 @@
         <v>2.7351399999999999</v>
       </c>
       <c r="AB108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="AC108">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>4.1599999999997195E-3</v>
       </c>
       <c r="AD108">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>414986376.3564654</v>
       </c>
       <c r="AE108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.4097176605648834E-9</v>
       </c>
       <c r="AF108">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19.843756249599409</v>
       </c>
-    </row>
-    <row r="109" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH108" s="3">
+        <f t="shared" si="19"/>
+        <v>2357304.5477321181</v>
+      </c>
+    </row>
+    <row r="109" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y109">
         <v>14</v>
       </c>
@@ -4922,27 +5311,31 @@
         <v>2.73489</v>
       </c>
       <c r="AB109">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>2.2799999999999999E-3</v>
       </c>
       <c r="AC109">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>3.909999999999858E-3</v>
       </c>
       <c r="AD109">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>355832616.56882244</v>
       </c>
       <c r="AE109">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.8103101105308248E-9</v>
       </c>
       <c r="AF109">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19.689971000070422</v>
       </c>
-    </row>
-    <row r="110" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH109" s="3">
+        <f t="shared" si="19"/>
+        <v>2215639.6109694396</v>
+      </c>
+    </row>
+    <row r="110" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y110">
         <v>15</v>
       </c>
@@ -4954,27 +5347,31 @@
         <v>2.73448</v>
       </c>
       <c r="AB110">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>2.3999999999999998E-3</v>
       </c>
       <c r="AC110">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>3.4999999999998366E-3</v>
       </c>
       <c r="AD110">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>302594232.75992894</v>
       </c>
       <c r="AE110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>3.3047556487746286E-9</v>
       </c>
       <c r="AF110">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19.527903300180952</v>
       </c>
-    </row>
-    <row r="113" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH110" s="3">
+        <f t="shared" si="19"/>
+        <v>1983309.114678506</v>
+      </c>
+    </row>
+    <row r="113" spans="21:34" x14ac:dyDescent="0.3">
       <c r="U113" t="s">
         <v>1</v>
       </c>
@@ -5008,8 +5405,11 @@
       <c r="AF113" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="114" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH113" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="21:34" x14ac:dyDescent="0.3">
       <c r="U114" s="1">
         <v>5</v>
       </c>
@@ -5033,27 +5433,31 @@
         <v>2.7519200000000001</v>
       </c>
       <c r="AB114">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>4.3000000000000002E-5</v>
       </c>
       <c r="AC114">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.0939999999999959E-2</v>
       </c>
       <c r="AD114">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>101044357219.82504</v>
       </c>
       <c r="AE114">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>9.8966436871330673E-12</v>
       </c>
       <c r="AF114">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>25.338825437770495</v>
       </c>
-    </row>
-    <row r="115" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH114" s="3">
+        <f>0.271/0.64 * $U$11 * AC114 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>11865855.103248507</v>
+      </c>
+    </row>
+    <row r="115" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y115">
         <v>2</v>
       </c>
@@ -5065,27 +5469,31 @@
         <v>2.7504200000000001</v>
       </c>
       <c r="AB115">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="AC115">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.9439999999999902E-2</v>
       </c>
       <c r="AD115">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>80673351563.701904</v>
       </c>
       <c r="AE115">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.2395666978213648E-11</v>
       </c>
       <c r="AF115">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>25.113674141625811</v>
       </c>
-    </row>
-    <row r="116" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH115" s="3">
+        <f t="shared" ref="AH115:AH128" si="20">0.271/0.64 * $U$11 * AC115 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * $X$5 /$U$13^2</f>
+        <v>11015865.482671933</v>
+      </c>
+    </row>
+    <row r="116" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y116">
         <v>3</v>
       </c>
@@ -5097,27 +5505,31 @@
         <v>2.7496399999999999</v>
       </c>
       <c r="AB116">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="AC116">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.8659999999999677E-2</v>
       </c>
       <c r="AD116">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>64530381523.433601</v>
       </c>
       <c r="AE116">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.5496576595271787E-11</v>
       </c>
       <c r="AF116">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>24.890401981218748</v>
       </c>
-    </row>
-    <row r="117" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH116" s="3">
+        <f t="shared" si="20"/>
+        <v>10573870.879972002</v>
+      </c>
+    </row>
+    <row r="117" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y117">
         <v>4</v>
       </c>
@@ -5129,27 +5541,31 @@
         <v>2.7479499999999999</v>
       </c>
       <c r="AB117">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>7.3999999999999996E-5</v>
       </c>
       <c r="AC117">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.6969999999999708E-2</v>
       </c>
       <c r="AD117">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>47583235180.875496</v>
       </c>
       <c r="AE117">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.1015805171690319E-11</v>
       </c>
       <c r="AF117">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>24.585746334063618</v>
       </c>
-    </row>
-    <row r="118" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH117" s="3">
+        <f t="shared" si="20"/>
+        <v>9616215.9074557815</v>
+      </c>
+    </row>
+    <row r="118" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y118">
         <v>5</v>
       </c>
@@ -5161,27 +5577,31 @@
         <v>2.7452899999999998</v>
       </c>
       <c r="AB118">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>9.2E-5</v>
       </c>
       <c r="AC118">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.4309999999999601E-2</v>
       </c>
       <c r="AD118">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>32274212204.680729</v>
       </c>
       <c r="AE118">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>3.0984489835354371E-11</v>
       </c>
       <c r="AF118">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>24.19753436454096</v>
       </c>
-    </row>
-    <row r="119" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH118" s="3">
+        <f t="shared" si="20"/>
+        <v>8108900.9802999869</v>
+      </c>
+    </row>
+    <row r="119" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y119">
         <v>6</v>
       </c>
@@ -5193,27 +5613,31 @@
         <v>2.7431100000000002</v>
       </c>
       <c r="AB119">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.15E-4</v>
       </c>
       <c r="AC119">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.2129999999999974E-2</v>
       </c>
       <c r="AD119">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>21886020631.322842</v>
       </c>
       <c r="AE119">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>4.5691266441045917E-11</v>
       </c>
       <c r="AF119">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>23.809113942614374</v>
       </c>
-    </row>
-    <row r="120" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH119" s="3">
+        <f t="shared" si="20"/>
+        <v>6873582.731728957</v>
+      </c>
+    </row>
+    <row r="120" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y120">
         <v>7</v>
       </c>
@@ -5225,27 +5649,31 @@
         <v>2.7412299999999998</v>
       </c>
       <c r="AB120">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.44E-4</v>
       </c>
       <c r="AC120">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.0249999999999648E-2</v>
       </c>
       <c r="AD120">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>14769480408.520527</v>
       </c>
       <c r="AE120">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>6.7707188901723257E-11</v>
       </c>
       <c r="AF120">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>23.415828754030052</v>
       </c>
-    </row>
-    <row r="121" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH120" s="3">
+        <f t="shared" si="20"/>
+        <v>5808262.4072728399</v>
+      </c>
+    </row>
+    <row r="121" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y121">
         <v>8</v>
       </c>
@@ -5257,27 +5685,31 @@
         <v>2.7386599999999999</v>
       </c>
       <c r="AB121">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.9000000000000001E-4</v>
       </c>
       <c r="AC121">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>7.6799999999996871E-3</v>
       </c>
       <c r="AD121">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>8387093080.0466805</v>
       </c>
       <c r="AE121">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.1923082174669681E-10</v>
       </c>
       <c r="AF121">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>22.849959823020722</v>
       </c>
-    </row>
-    <row r="122" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH121" s="3">
+        <f t="shared" si="20"/>
+        <v>4351946.8573517194</v>
+      </c>
+    </row>
+    <row r="122" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y122">
         <v>9</v>
       </c>
@@ -5289,27 +5721,31 @@
         <v>2.73672</v>
       </c>
       <c r="AB122">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>2.4800000000000001E-4</v>
       </c>
       <c r="AC122">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>5.7399999999998563E-3</v>
       </c>
       <c r="AD122">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>4802463307.0286531</v>
       </c>
       <c r="AE122">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.0822647380490098E-10</v>
       </c>
       <c r="AF122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>22.292394812188135</v>
       </c>
-    </row>
-    <row r="123" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH122" s="3">
+        <f t="shared" si="20"/>
+        <v>3252626.94807282</v>
+      </c>
+    </row>
+    <row r="123" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y123">
         <v>10</v>
       </c>
@@ -5321,27 +5757,31 @@
         <v>2.7351100000000002</v>
       </c>
       <c r="AB123">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>3.2400000000000001E-4</v>
       </c>
       <c r="AC123">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>4.129999999999967E-3</v>
       </c>
       <c r="AD123">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>2644897738.198</v>
       </c>
       <c r="AE123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>3.7808645134284541E-10</v>
       </c>
       <c r="AF123">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>21.695898239202272</v>
       </c>
-    </row>
-    <row r="124" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH123" s="3">
+        <f t="shared" si="20"/>
+        <v>2340304.7553207269</v>
+      </c>
+    </row>
+    <row r="124" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y124">
         <v>11</v>
       </c>
@@ -5353,27 +5793,31 @@
         <v>2.7339000000000002</v>
       </c>
       <c r="AB124">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>4.1599999999999997E-4</v>
       </c>
       <c r="AC124">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.9200000000000337E-3</v>
       </c>
       <c r="AD124">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>1456442570.8665562</v>
       </c>
       <c r="AE124">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>6.8660448410610428E-10</v>
       </c>
       <c r="AF124">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>21.099262704040608</v>
       </c>
-    </row>
-    <row r="125" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH124" s="3">
+        <f t="shared" si="20"/>
+        <v>1654646.461389021</v>
+      </c>
+    </row>
+    <row r="125" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y125">
         <v>12</v>
       </c>
@@ -5385,27 +5829,31 @@
         <v>2.73325</v>
       </c>
       <c r="AB125">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="AC125">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.2699999999997722E-3</v>
       </c>
       <c r="AD125">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>942019074.32914531</v>
       </c>
       <c r="AE125">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.0615496302048295E-9</v>
       </c>
       <c r="AF125">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>20.663536081092687</v>
       </c>
-    </row>
-    <row r="126" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH125" s="3">
+        <f t="shared" si="20"/>
+        <v>1286317.6258057051</v>
+      </c>
+    </row>
+    <row r="126" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y126">
         <v>13</v>
       </c>
@@ -5417,27 +5865,31 @@
         <v>2.7326800000000002</v>
       </c>
       <c r="AB126">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="AC126">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.7000000000000348E-3</v>
       </c>
       <c r="AD126">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>587897366.50504434</v>
       </c>
       <c r="AE126">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.7009771721632974E-9</v>
       </c>
       <c r="AF126">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>20.192062943867715</v>
       </c>
-    </row>
-    <row r="127" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH126" s="3">
+        <f t="shared" si="20"/>
+        <v>963321.5699867676</v>
+      </c>
+    </row>
+    <row r="127" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y127">
         <v>14</v>
       </c>
@@ -5449,27 +5901,31 @@
         <v>2.7322799999999998</v>
       </c>
       <c r="AB127">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="AC127">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.2999999999996348E-3</v>
       </c>
       <c r="AD127">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>385344492.33092141</v>
       </c>
       <c r="AE127">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.5950805575319661E-9</v>
       </c>
       <c r="AF127">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19.769648277445476</v>
       </c>
-    </row>
-    <row r="128" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="AH127" s="3">
+        <f t="shared" si="20"/>
+        <v>736657.67116612964</v>
+      </c>
+    </row>
+    <row r="128" spans="21:34" x14ac:dyDescent="0.3">
       <c r="Y128">
         <v>15</v>
       </c>
@@ -5481,24 +5937,28 @@
         <v>2.7319900000000001</v>
       </c>
       <c r="AB128">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="AC128">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.0099999999999554E-3</v>
       </c>
       <c r="AD128">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>261960150.07502484</v>
       </c>
       <c r="AE128">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>3.8173745117858652E-9</v>
       </c>
       <c r="AF128">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19.383702951206867</v>
+      </c>
+      <c r="AH128" s="3">
+        <f t="shared" si="20"/>
+        <v>572326.34452151321</v>
       </c>
     </row>
   </sheetData>
@@ -5508,24 +5968,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
04: Coefficients, graphs, tex table
</commit_message>
<xml_diff>
--- a/04_RozpadPlazmatu/data/RozpadPlazmatu.xlsx
+++ b/04_RozpadPlazmatu/data/RozpadPlazmatu.xlsx
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG21" sqref="AG21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
01; 03; 04 Konzultace
</commit_message>
<xml_diff>
--- a/04_RozpadPlazmatu/data/RozpadPlazmatu.xlsx
+++ b/04_RozpadPlazmatu/data/RozpadPlazmatu.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\PraktikumPlazma\04_RozpadPlazmatu\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FF6D32-3328-4927-B841-41EFDA5374CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="19176"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -99,7 +105,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000000"/>
   </numFmts>
@@ -149,7 +155,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -165,7 +171,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -207,7 +213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,9 +246,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,6 +298,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -450,36 +490,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+      <selection activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.33203125" customWidth="1"/>
-    <col min="29" max="29" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.28515625" customWidth="1"/>
+    <col min="29" max="29" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="9.44140625" customWidth="1"/>
+    <col min="34" max="34" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="9.42578125" customWidth="1"/>
     <col min="37" max="37" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -487,7 +527,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -549,7 +589,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -611,19 +651,19 @@
         <v>16.967892430370664</v>
       </c>
       <c r="AK5" s="3">
-        <f>0.271/0.64 * $U$11 * AC5 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * AA5 /$U$13^2</f>
-        <v>23745290.718660593</v>
+        <f>0.271/0.64 * $U$11 * AC5 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * AA5*1000000000 /$U$13^2</f>
+        <v>2.3745290718660596E+16</v>
       </c>
       <c r="AL5">
         <f>1/AK5</f>
-        <v>4.2113613678106495E-8</v>
+        <v>4.2113613678106494E-17</v>
       </c>
       <c r="AM5">
         <f>LN(AK5)</f>
-        <v>16.98289478325367</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+        <v>37.70616062020008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -673,19 +713,19 @@
         <v>16.94535350468276</v>
       </c>
       <c r="AK6" s="3">
-        <f t="shared" ref="AK6:AK19" si="7">0.271/0.64 * $U$11 * AC6 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * AA6 /$U$13^2</f>
-        <v>23208379.187001254</v>
+        <f t="shared" ref="AK6:AK19" si="7">0.271/0.64 * $U$11 * AC6 * 1000000000 * 8 * PI()^2 * $V$11 *$W$11 * AA6*1000000000 /$U$13^2</f>
+        <v>2.3208379187001256E+16</v>
       </c>
       <c r="AL6">
         <f t="shared" ref="AL6:AL19" si="8">1/AK6</f>
-        <v>4.3087886144159884E-8</v>
+        <v>4.3087886144159882E-17</v>
       </c>
       <c r="AM6">
         <f t="shared" ref="AM6:AM19" si="9">LN(AK6)</f>
-        <v>16.960023943283186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+        <v>37.6832897802296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1</v>
       </c>
@@ -775,18 +815,18 @@
       </c>
       <c r="AK7" s="3">
         <f t="shared" si="7"/>
-        <v>21867637.052404951</v>
+        <v>2.1867637052404948E+16</v>
       </c>
       <c r="AL7">
         <f t="shared" si="8"/>
-        <v>4.5729677953019724E-8</v>
+        <v>4.5729677953019733E-17</v>
       </c>
       <c r="AM7">
         <f t="shared" si="9"/>
-        <v>16.900518341658127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+        <v>37.623784178604538</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -900,18 +940,18 @@
       </c>
       <c r="AK8" s="3">
         <f t="shared" si="7"/>
-        <v>20273270.516078338</v>
+        <v>2.0273270516078336E+16</v>
       </c>
       <c r="AL8">
         <f t="shared" si="8"/>
-        <v>4.9326032482372265E-8</v>
+        <v>4.9326032482372266E-17</v>
       </c>
       <c r="AM8">
         <f t="shared" si="9"/>
-        <v>16.824813853024224</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+        <v>37.548079689970635</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1012,18 +1052,18 @@
       </c>
       <c r="AK9" s="3">
         <f t="shared" si="7"/>
-        <v>18594997.199588377</v>
+        <v>1.8594997199588376E+16</v>
       </c>
       <c r="AL9">
         <f t="shared" si="8"/>
-        <v>5.3777905383182108E-8</v>
+        <v>5.3777905383182113E-17</v>
       </c>
       <c r="AM9">
         <f t="shared" si="9"/>
-        <v>16.738403134741048</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+        <v>37.461668971687459</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="U10" t="s">
         <v>15</v>
       </c>
@@ -1077,18 +1117,18 @@
       </c>
       <c r="AK10" s="3">
         <f t="shared" si="7"/>
-        <v>16306769.478873594</v>
+        <v>1.6306769478873594E+16</v>
       </c>
       <c r="AL10">
         <f t="shared" si="8"/>
-        <v>6.1324224966542909E-8</v>
+        <v>6.1324224966542912E-17</v>
       </c>
       <c r="AM10">
         <f t="shared" si="9"/>
-        <v>16.607090885013918</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+        <v>37.330356721960328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1149,18 +1189,18 @@
       </c>
       <c r="AK11" s="3">
         <f t="shared" si="7"/>
-        <v>13684753.587385593</v>
+        <v>1.3684753587385594E+16</v>
       </c>
       <c r="AL11">
         <f t="shared" si="8"/>
-        <v>7.307402311736073E-8</v>
+        <v>7.307402311736072E-17</v>
       </c>
       <c r="AM11">
         <f t="shared" si="9"/>
-        <v>16.431792894257949</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+        <v>37.155058731204356</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1214,18 +1254,18 @@
       </c>
       <c r="AK12" s="3">
         <f t="shared" si="7"/>
-        <v>11214981.818105029</v>
+        <v>1.1214981818105028E+16</v>
       </c>
       <c r="AL12">
         <f t="shared" si="8"/>
-        <v>8.9166439698157957E-8</v>
+        <v>8.9166439698157969E-17</v>
       </c>
       <c r="AM12">
         <f t="shared" si="9"/>
-        <v>16.232761104722918</v>
-      </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+        <v>36.956026941669329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1279,18 +1319,18 @@
       </c>
       <c r="AK13" s="3">
         <f t="shared" si="7"/>
-        <v>8821614.560030181</v>
+        <v>8821614560030181</v>
       </c>
       <c r="AL13">
         <f t="shared" si="8"/>
-        <v>1.1335793387878179E-7</v>
+        <v>1.133579338787818E-16</v>
       </c>
       <c r="AM13">
         <f t="shared" si="9"/>
-        <v>15.992715467922906</v>
-      </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+        <v>36.715981304869317</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1341,18 +1381,18 @@
       </c>
       <c r="AK14" s="3">
         <f t="shared" si="7"/>
-        <v>6561171.2146784114</v>
+        <v>6561171214678411</v>
       </c>
       <c r="AL14">
         <f t="shared" si="8"/>
-        <v>1.5241181296455679E-7</v>
+        <v>1.524118129645568E-16</v>
       </c>
       <c r="AM14">
         <f t="shared" si="9"/>
-        <v>15.696679683807041</v>
-      </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+        <v>36.419945520753451</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1</v>
       </c>
@@ -1442,18 +1482,18 @@
       </c>
       <c r="AK15" s="3">
         <f t="shared" si="7"/>
-        <v>4905727.0664768312</v>
+        <v>4905727066476831</v>
       </c>
       <c r="AL15">
         <f t="shared" si="8"/>
-        <v>2.0384338273392259E-7</v>
+        <v>2.0384338273392261E-16</v>
       </c>
       <c r="AM15">
         <f t="shared" si="9"/>
-        <v>15.405913869655555</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+        <v>36.129179706601967</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1561,18 +1601,18 @@
       </c>
       <c r="AK16" s="3">
         <f t="shared" si="7"/>
-        <v>3498497.4953556373</v>
+        <v>3498497495355637</v>
       </c>
       <c r="AL16">
         <f t="shared" si="8"/>
-        <v>2.8583699183078756E-7</v>
+        <v>2.8583699183078758E-16</v>
       </c>
       <c r="AM16">
         <f t="shared" si="9"/>
-        <v>15.067844147248335</v>
-      </c>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+        <v>35.791109984194748</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1665,18 +1705,18 @@
       </c>
       <c r="AK17" s="3">
         <f t="shared" si="7"/>
-        <v>2423420.322458623</v>
+        <v>2423420322458623</v>
       </c>
       <c r="AL17">
         <f t="shared" si="8"/>
-        <v>4.1263993321037846E-7</v>
+        <v>4.1263993321037846E-16</v>
       </c>
       <c r="AM17">
         <f t="shared" si="9"/>
-        <v>14.700690456672689</v>
-      </c>
-    </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+        <v>35.423956293619099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y18">
         <v>14</v>
       </c>
@@ -1721,18 +1761,18 @@
       </c>
       <c r="AK18" s="3">
         <f t="shared" si="7"/>
-        <v>1673451.9632705331</v>
+        <v>1673451963270533</v>
       </c>
       <c r="AL18">
         <f t="shared" si="8"/>
-        <v>5.9756719759414948E-7</v>
+        <v>5.9756719759414954E-16</v>
       </c>
       <c r="AM18">
         <f t="shared" si="9"/>
-        <v>14.330399094871694</v>
-      </c>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+        <v>35.053664931818105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y19">
         <v>15</v>
       </c>
@@ -1777,18 +1817,18 @@
       </c>
       <c r="AK19" s="3">
         <f t="shared" si="7"/>
-        <v>1281710.8205430964</v>
+        <v>1281710820543096.5</v>
       </c>
       <c r="AL19">
         <f t="shared" si="8"/>
-        <v>7.8020719180343055E-7</v>
+        <v>7.8020719180343052E-16</v>
       </c>
       <c r="AM19">
         <f t="shared" si="9"/>
-        <v>14.063706322019094</v>
-      </c>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+        <v>34.786972158965504</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1796,7 +1836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1804,7 +1844,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1863,7 +1903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1937,7 +1977,7 @@
         <v>16.989022894788956</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1</v>
       </c>
@@ -2041,7 +2081,7 @@
         <v>16.921347813345804</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -2164,7 +2204,7 @@
         <v>16.889270105887629</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -2271,7 +2311,7 @@
         <v>16.806004238475644</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y27">
         <v>5</v>
       </c>
@@ -2327,7 +2367,7 @@
         <v>16.71153558494991</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y28">
         <v>6</v>
       </c>
@@ -2383,7 +2423,7 @@
         <v>16.53431574222228</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2445,7 +2485,7 @@
         <v>16.318239671859939</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -2507,7 +2547,7 @@
         <v>15.973698320324775</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -2569,7 +2609,7 @@
         <v>15.683530082306232</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -2631,7 +2671,7 @@
         <v>15.299334084872589</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>1</v>
       </c>
@@ -2732,7 +2772,7 @@
         <v>14.988305891017912</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -2851,7 +2891,7 @@
         <v>14.72387619760077</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2955,7 +2995,7 @@
         <v>14.463660282086531</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y36">
         <v>14</v>
       </c>
@@ -3011,7 +3051,7 @@
         <v>14.203977340517522</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y37">
         <v>15</v>
       </c>
@@ -3067,7 +3107,7 @@
         <v>13.921176216107925</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -3075,7 +3115,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -3083,7 +3123,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -3142,7 +3182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -3216,7 +3256,7 @@
         <v>16.692136197669118</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>1</v>
       </c>
@@ -3317,7 +3357,7 @@
         <v>16.422055603722406</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -3436,7 +3476,7 @@
         <v>16.443105966751453</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -3540,7 +3580,7 @@
         <v>16.325282317495638</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y45">
         <v>5</v>
       </c>
@@ -3596,7 +3636,7 @@
         <v>16.145573251420693</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y46">
         <v>6</v>
       </c>
@@ -3652,7 +3692,7 @@
         <v>15.927651422359848</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -3717,7 +3757,7 @@
         <v>15.680879457992823</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -3779,7 +3819,7 @@
         <v>15.401253499831478</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -3841,7 +3881,7 @@
         <v>15.172803504979951</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -3903,7 +3943,7 @@
         <v>14.898075202714708</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>1</v>
       </c>
@@ -4004,7 +4044,7 @@
         <v>14.688893477448191</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -4123,7 +4163,7 @@
         <v>14.448694034602033</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -4227,7 +4267,7 @@
         <v>14.21925944536717</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y54">
         <v>14</v>
       </c>
@@ -4283,7 +4323,7 @@
         <v>13.970974315628791</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y55">
         <v>15</v>
       </c>
@@ -4339,7 +4379,7 @@
         <v>13.711830364596146</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -4401,7 +4441,7 @@
         <v>13.44681179427381</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -4409,7 +4449,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -4417,7 +4457,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -4476,7 +4516,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>1</v>
       </c>
@@ -4589,7 +4629,7 @@
         <v>17.051374388402497</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -4708,7 +4748,7 @@
         <v>17.027873392116074</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -4812,7 +4852,7 @@
         <v>17.013177165382135</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y63">
         <v>4</v>
       </c>
@@ -4868,7 +4908,7 @@
         <v>16.9542259362895</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
       <c r="Y64">
         <v>5</v>
       </c>
@@ -4924,7 +4964,7 @@
         <v>16.890615657825119</v>
       </c>
     </row>
-    <row r="65" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="65" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y65">
         <v>6</v>
       </c>
@@ -4980,7 +5020,7 @@
         <v>16.794550546890214</v>
       </c>
     </row>
-    <row r="66" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="66" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y66">
         <v>7</v>
       </c>
@@ -5036,7 +5076,7 @@
         <v>16.673691874388453</v>
       </c>
     </row>
-    <row r="67" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="67" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y67">
         <v>8</v>
       </c>
@@ -5092,7 +5132,7 @@
         <v>16.507682763178781</v>
       </c>
     </row>
-    <row r="68" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="68" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y68">
         <v>9</v>
       </c>
@@ -5148,7 +5188,7 @@
         <v>16.362491199327259</v>
       </c>
     </row>
-    <row r="69" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="69" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y69">
         <v>10</v>
       </c>
@@ -5204,7 +5244,7 @@
         <v>16.17583842734696</v>
       </c>
     </row>
-    <row r="70" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="70" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y70">
         <v>11</v>
       </c>
@@ -5260,7 +5300,7 @@
         <v>15.994662500042113</v>
       </c>
     </row>
-    <row r="71" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="71" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y71">
         <v>12</v>
       </c>
@@ -5316,7 +5356,7 @@
         <v>15.751759592888751</v>
       </c>
     </row>
-    <row r="72" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="72" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y72">
         <v>13</v>
       </c>
@@ -5372,7 +5412,7 @@
         <v>15.522150632015993</v>
       </c>
     </row>
-    <row r="73" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="73" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y73">
         <v>14</v>
       </c>
@@ -5428,7 +5468,7 @@
         <v>15.277121267818627</v>
       </c>
     </row>
-    <row r="74" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="74" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y74">
         <v>15</v>
       </c>
@@ -5484,7 +5524,7 @@
         <v>14.965146247026659</v>
       </c>
     </row>
-    <row r="77" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="77" spans="21:39" x14ac:dyDescent="0.25">
       <c r="U77" t="s">
         <v>1</v>
       </c>
@@ -5537,7 +5577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="78" spans="21:39" x14ac:dyDescent="0.25">
       <c r="U78" s="1">
         <v>200</v>
       </c>
@@ -5605,7 +5645,7 @@
         <v>16.966539116980716</v>
       </c>
     </row>
-    <row r="79" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="79" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y79">
         <v>2</v>
       </c>
@@ -5661,7 +5701,7 @@
         <v>16.91794906355069</v>
       </c>
     </row>
-    <row r="80" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="80" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y80">
         <v>3</v>
       </c>
@@ -5717,7 +5757,7 @@
         <v>16.839051604434246</v>
       </c>
     </row>
-    <row r="81" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="81" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y81">
         <v>4</v>
       </c>
@@ -5773,7 +5813,7 @@
         <v>16.784161453569318</v>
       </c>
     </row>
-    <row r="82" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="82" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y82">
         <v>5</v>
       </c>
@@ -5829,7 +5869,7 @@
         <v>16.672694330372522</v>
       </c>
     </row>
-    <row r="83" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="83" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y83">
         <v>6</v>
       </c>
@@ -5885,7 +5925,7 @@
         <v>16.516250268229889</v>
       </c>
     </row>
-    <row r="84" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="84" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y84">
         <v>7</v>
       </c>
@@ -5941,7 +5981,7 @@
         <v>16.308297188146586</v>
       </c>
     </row>
-    <row r="85" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="85" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y85">
         <v>8</v>
       </c>
@@ -5997,7 +6037,7 @@
         <v>16.080401586985708</v>
       </c>
     </row>
-    <row r="86" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="86" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y86">
         <v>9</v>
       </c>
@@ -6053,7 +6093,7 @@
         <v>15.856622769680001</v>
       </c>
     </row>
-    <row r="87" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="87" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y87">
         <v>10</v>
       </c>
@@ -6109,7 +6149,7 @@
         <v>15.623543111664144</v>
       </c>
     </row>
-    <row r="88" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="88" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y88">
         <v>11</v>
       </c>
@@ -6165,7 +6205,7 @@
         <v>15.389507261413534</v>
       </c>
     </row>
-    <row r="89" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="89" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y89">
         <v>12</v>
       </c>
@@ -6221,7 +6261,7 @@
         <v>15.121693756138837</v>
       </c>
     </row>
-    <row r="90" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="90" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y90">
         <v>13</v>
       </c>
@@ -6277,7 +6317,7 @@
         <v>14.844656882594387</v>
       </c>
     </row>
-    <row r="91" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="91" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y91">
         <v>14</v>
       </c>
@@ -6333,7 +6373,7 @@
         <v>14.735271163612236</v>
       </c>
     </row>
-    <row r="92" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="92" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y92">
         <v>15</v>
       </c>
@@ -6389,7 +6429,7 @@
         <v>14.596996215077962</v>
       </c>
     </row>
-    <row r="95" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="95" spans="21:39" x14ac:dyDescent="0.25">
       <c r="U95" t="s">
         <v>1</v>
       </c>
@@ -6442,7 +6482,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="96" spans="21:39" x14ac:dyDescent="0.25">
       <c r="U96" s="1">
         <v>450</v>
       </c>
@@ -6510,7 +6550,7 @@
         <v>16.907155718424665</v>
       </c>
     </row>
-    <row r="97" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="97" spans="21:39" x14ac:dyDescent="0.25">
       <c r="U97" t="s">
         <v>7</v>
       </c>
@@ -6569,7 +6609,7 @@
         <v>16.824240211327737</v>
       </c>
     </row>
-    <row r="98" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="98" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y98">
         <v>3</v>
       </c>
@@ -6625,7 +6665,7 @@
         <v>16.778777188395981</v>
       </c>
     </row>
-    <row r="99" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="99" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y99">
         <v>4</v>
       </c>
@@ -6681,7 +6721,7 @@
         <v>16.614865643801238</v>
       </c>
     </row>
-    <row r="100" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="100" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y100">
         <v>5</v>
       </c>
@@ -6737,7 +6777,7 @@
         <v>16.479932971868315</v>
       </c>
     </row>
-    <row r="101" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="101" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y101">
         <v>6</v>
       </c>
@@ -6793,7 +6833,7 @@
         <v>16.374151591206278</v>
       </c>
     </row>
-    <row r="102" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="102" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y102">
         <v>7</v>
       </c>
@@ -6849,7 +6889,7 @@
         <v>16.177463543518289</v>
       </c>
     </row>
-    <row r="103" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="103" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y103">
         <v>8</v>
       </c>
@@ -6905,7 +6945,7 @@
         <v>15.957684905290758</v>
       </c>
     </row>
-    <row r="104" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="104" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y104">
         <v>9</v>
       </c>
@@ -6961,7 +7001,7 @@
         <v>15.662127368415176</v>
       </c>
     </row>
-    <row r="105" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="105" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y105">
         <v>10</v>
       </c>
@@ -7017,7 +7057,7 @@
         <v>15.409395037538381</v>
       </c>
     </row>
-    <row r="106" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="106" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y106">
         <v>11</v>
       </c>
@@ -7073,7 +7113,7 @@
         <v>15.184460762876695</v>
       </c>
     </row>
-    <row r="107" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="107" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y107">
         <v>12</v>
       </c>
@@ -7129,7 +7169,7 @@
         <v>14.99707312342392</v>
       </c>
     </row>
-    <row r="108" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="108" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y108">
         <v>13</v>
       </c>
@@ -7185,7 +7225,7 @@
         <v>14.674551487194185</v>
       </c>
     </row>
-    <row r="109" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="109" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y109">
         <v>14</v>
       </c>
@@ -7241,7 +7281,7 @@
         <v>14.61248237974133</v>
       </c>
     </row>
-    <row r="110" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="110" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y110">
         <v>15</v>
       </c>
@@ -7297,7 +7337,7 @@
         <v>14.501558048379298</v>
       </c>
     </row>
-    <row r="113" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="113" spans="21:39" x14ac:dyDescent="0.25">
       <c r="U113" t="s">
         <v>1</v>
       </c>
@@ -7350,7 +7390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="114" spans="21:39" x14ac:dyDescent="0.25">
       <c r="U114" s="1">
         <v>5</v>
       </c>
@@ -7418,7 +7458,7 @@
         <v>16.296813845380907</v>
       </c>
     </row>
-    <row r="115" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="115" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y115">
         <v>2</v>
       </c>
@@ -7474,7 +7514,7 @@
         <v>16.221940216379267</v>
       </c>
     </row>
-    <row r="116" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="116" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y116">
         <v>3</v>
       </c>
@@ -7530,7 +7570,7 @@
         <v>16.180705979494803</v>
       </c>
     </row>
-    <row r="117" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="117" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y117">
         <v>4</v>
       </c>
@@ -7586,7 +7626,7 @@
         <v>16.085156048447139</v>
       </c>
     </row>
-    <row r="118" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="118" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y118">
         <v>5</v>
       </c>
@@ -7642,7 +7682,7 @@
         <v>15.913699099637245</v>
       </c>
     </row>
-    <row r="119" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="119" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y119">
         <v>6</v>
       </c>
@@ -7698,7 +7738,7 @@
         <v>15.747627826242768</v>
       </c>
     </row>
-    <row r="120" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="120" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y120">
         <v>7</v>
       </c>
@@ -7754,7 +7794,7 @@
         <v>15.578538220423491</v>
       </c>
     </row>
-    <row r="121" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="121" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y121">
         <v>8</v>
       </c>
@@ -7810,7 +7850,7 @@
         <v>15.288942086897533</v>
       </c>
     </row>
-    <row r="122" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="122" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y122">
         <v>9</v>
       </c>
@@ -7866,7 +7906,7 @@
         <v>14.99707312342392</v>
       </c>
     </row>
-    <row r="123" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="123" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y123">
         <v>10</v>
       </c>
@@ -7922,7 +7962,7 @@
         <v>14.667302851473924</v>
       </c>
     </row>
-    <row r="124" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="124" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y124">
         <v>11</v>
       </c>
@@ -7978,7 +8018,7 @@
         <v>14.32016656752565</v>
       </c>
     </row>
-    <row r="125" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="125" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y125">
         <v>12</v>
       </c>
@@ -8034,7 +8074,7 @@
         <v>14.068124998883063</v>
       </c>
     </row>
-    <row r="126" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="126" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y126">
         <v>13</v>
       </c>
@@ -8090,7 +8130,7 @@
         <v>13.778764853760558</v>
       </c>
     </row>
-    <row r="127" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="127" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y127">
         <v>14</v>
       </c>
@@ -8146,7 +8186,7 @@
         <v>13.510354480000542</v>
       </c>
     </row>
-    <row r="128" spans="21:39" x14ac:dyDescent="0.3">
+    <row r="128" spans="21:39" x14ac:dyDescent="0.25">
       <c r="Y128">
         <v>15</v>
       </c>
@@ -8209,24 +8249,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>